<commit_message>
add thư viện pom
</commit_message>
<xml_diff>
--- a/datatest/Login.xlsx
+++ b/datatest/Login.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ngan.dang/Testing/MiniAppCenter/datatest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED392C83-0687-004A-BDEC-05B626F4B308}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F819DD92-C853-984F-8D0A-0A0450979035}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15900" yWindow="12140" windowWidth="19200" windowHeight="11320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7400" yWindow="12580" windowWidth="19200" windowHeight="11320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SheetLogin" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>username</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>MiniApp Admin</t>
-  </si>
-  <si>
-    <t>119411Ngan@@@</t>
   </si>
   <si>
     <t xml:space="preserve">Momo@2022
@@ -91,7 +88,7 @@
     <t>0967313471</t>
   </si>
   <si>
-    <t>0967313400</t>
+    <t>0967313500</t>
   </si>
 </sst>
 </file>
@@ -422,7 +419,7 @@
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -509,9 +506,7 @@
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -591,7 +586,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="3">
         <v>12345678</v>
@@ -625,7 +620,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -641,10 +636,10 @@
     </row>
     <row r="13" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="2"/>
@@ -659,7 +654,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="2">
         <v>12345678</v>

</xml_diff>